<commit_message>
Phase-2 changes scripts modified
Phase-2 changes scripts modified
</commit_message>
<xml_diff>
--- a/Access_Desktop.suite/Resources/Sanity_testdata.xlsx
+++ b/Access_Desktop.suite/Resources/Sanity_testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/suganthinatrajan/Eggplant_Testcases/Access_Desktop.suite/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E63C4A28-14A2-EE45-BD00-0F7AE2DDDEFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BE0B32C-5B03-E441-9BC9-B990E895046F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19260" activeTab="2" xr2:uid="{662A243E-2B0E-4C05-8B32-EC5026EB9CF6}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19260" activeTab="1" xr2:uid="{662A243E-2B0E-4C05-8B32-EC5026EB9CF6}"/>
   </bookViews>
   <sheets>
     <sheet name="CR" sheetId="3" r:id="rId1"/>
@@ -757,7 +757,7 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -922,8 +922,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA4FE13A-C238-440C-BD75-766A4748C928}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F6"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1064,7 +1064,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D738776A-5825-42F9-9F09-6439114E8738}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>

</xml_diff>